<commit_message>
Added model 232 - breast cancer signalling pathways MCF7 complete
</commit_message>
<xml_diff>
--- a/report/online_only_table_1.xlsx
+++ b/report/online_only_table_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="390">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1187,6 +1187,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.1371/journal.pone.0298788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-MCF7-COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -1423,13 +1426,13 @@
   </sheetPr>
   <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D215" activeCellId="0" sqref="D215"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="N216" activeCellId="0" sqref="N216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="49.49"/>
@@ -11171,13 +11174,25 @@
       </c>
       <c r="O215" s="3"/>
     </row>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1"/>
-      <c r="B216" s="2"/>
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
-      <c r="E216" s="3"/>
-      <c r="F216" s="2"/>
+    <row r="216" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C216" s="3" t="n">
+        <v>109</v>
+      </c>
+      <c r="D216" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E216" s="3" t="n">
+        <v>275</v>
+      </c>
+      <c r="F216" s="6" t="s">
+        <v>388</v>
+      </c>
       <c r="G216" s="3"/>
       <c r="H216" s="3"/>
       <c r="I216" s="3"/>
@@ -11185,7 +11200,9 @@
       <c r="K216" s="3"/>
       <c r="L216" s="3"/>
       <c r="M216" s="3"/>
-      <c r="N216" s="4"/>
+      <c r="N216" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="O216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24768,6 +24785,7 @@
     <hyperlink ref="F213" r:id="rId211" display="https://doi.org/10.3389/fmolb.2020.502573"/>
     <hyperlink ref="F214" r:id="rId212" display="https://doi.org/10.48550/arXiv.2202.11182"/>
     <hyperlink ref="F215" r:id="rId213" display="https://doi.org/10.1371/journal.pone.0298788"/>
+    <hyperlink ref="F216" r:id="rId214" display="https://doi.org/10.1371/journal.pone.0298788"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added model 234 - breast cancer signalling pathways MDAMB468 complete
</commit_message>
<xml_diff>
--- a/report/online_only_table_1.xlsx
+++ b/report/online_only_table_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="392">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1193,6 +1193,9 @@
   </si>
   <si>
     <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-T47D-COMPLETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-MDAMB468-COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -1432,10 +1435,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A217" activeCellId="0" sqref="A217:N217"/>
+      <selection pane="bottomLeft" activeCell="N219" activeCellId="0" sqref="N219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="49.49"/>
@@ -11239,13 +11242,25 @@
       </c>
       <c r="O217" s="3"/>
     </row>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1"/>
-      <c r="B218" s="2"/>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
-      <c r="E218" s="3"/>
-      <c r="F218" s="2"/>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C218" s="3" t="n">
+        <v>111</v>
+      </c>
+      <c r="D218" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E218" s="3" t="n">
+        <v>271</v>
+      </c>
+      <c r="F218" s="6" t="s">
+        <v>388</v>
+      </c>
       <c r="G218" s="3"/>
       <c r="H218" s="3"/>
       <c r="I218" s="3"/>
@@ -11253,7 +11268,9 @@
       <c r="K218" s="3"/>
       <c r="L218" s="3"/>
       <c r="M218" s="3"/>
-      <c r="N218" s="4"/>
+      <c r="N218" s="4" t="n">
+        <v>6</v>
+      </c>
       <c r="O218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24804,6 +24821,7 @@
     <hyperlink ref="F215" r:id="rId213" display="https://doi.org/10.1371/journal.pone.0298788"/>
     <hyperlink ref="F216" r:id="rId214" display="https://doi.org/10.1371/journal.pone.0298788"/>
     <hyperlink ref="F217" r:id="rId215" display="https://doi.org/10.1371/journal.pone.0298788"/>
+    <hyperlink ref="F218" r:id="rId216" display="https://doi.org/10.1371/journal.pone.0298788"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added model 235 - breast cancer signalling pathways MDAMB231 complete
</commit_message>
<xml_diff>
--- a/report/online_only_table_1.xlsx
+++ b/report/online_only_table_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="393">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1196,6 +1196,9 @@
   </si>
   <si>
     <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-MDAMB468-COMPLETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-MDAMB231-COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -1435,10 +1438,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N219" activeCellId="0" sqref="N219"/>
+      <selection pane="bottomLeft" activeCell="N220" activeCellId="0" sqref="N220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="49.49"/>
@@ -11273,13 +11276,25 @@
       </c>
       <c r="O218" s="3"/>
     </row>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1"/>
-      <c r="B219" s="2"/>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3"/>
-      <c r="E219" s="3"/>
-      <c r="F219" s="2"/>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C219" s="3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D219" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E219" s="3" t="n">
+        <v>270</v>
+      </c>
+      <c r="F219" s="6" t="s">
+        <v>388</v>
+      </c>
       <c r="G219" s="3"/>
       <c r="H219" s="3"/>
       <c r="I219" s="3"/>
@@ -11287,7 +11302,9 @@
       <c r="K219" s="3"/>
       <c r="L219" s="3"/>
       <c r="M219" s="3"/>
-      <c r="N219" s="4"/>
+      <c r="N219" s="4" t="n">
+        <v>7</v>
+      </c>
       <c r="O219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24822,6 +24839,7 @@
     <hyperlink ref="F216" r:id="rId214" display="https://doi.org/10.1371/journal.pone.0298788"/>
     <hyperlink ref="F217" r:id="rId215" display="https://doi.org/10.1371/journal.pone.0298788"/>
     <hyperlink ref="F218" r:id="rId216" display="https://doi.org/10.1371/journal.pone.0298788"/>
+    <hyperlink ref="F219" r:id="rId217" display="https://doi.org/10.1371/journal.pone.0298788"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added model 236 - breast cancer signalling pathways BT549 complete
</commit_message>
<xml_diff>
--- a/report/online_only_table_1.xlsx
+++ b/report/online_only_table_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="394">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1199,6 +1199,9 @@
   </si>
   <si>
     <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-MDAMB231-COMPLETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BREAST-CANCER-SIGNALLING-PATHWAYS-BT548-COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -1436,9 +1439,9 @@
   <dimension ref="A1:Q1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N220" activeCellId="0" sqref="N220"/>
+      <selection pane="bottomLeft" activeCell="N221" activeCellId="0" sqref="N221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11307,13 +11310,25 @@
       </c>
       <c r="O219" s="3"/>
     </row>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="1"/>
-      <c r="B220" s="2"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
-      <c r="E220" s="3"/>
-      <c r="F220" s="2"/>
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C220" s="3" t="n">
+        <v>109</v>
+      </c>
+      <c r="D220" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E220" s="3" t="n">
+        <v>263</v>
+      </c>
+      <c r="F220" s="6" t="s">
+        <v>388</v>
+      </c>
       <c r="G220" s="3"/>
       <c r="H220" s="3"/>
       <c r="I220" s="3"/>
@@ -11321,7 +11336,9 @@
       <c r="K220" s="3"/>
       <c r="L220" s="3"/>
       <c r="M220" s="3"/>
-      <c r="N220" s="4"/>
+      <c r="N220" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="O220" s="3"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24840,6 +24857,7 @@
     <hyperlink ref="F217" r:id="rId215" display="https://doi.org/10.1371/journal.pone.0298788"/>
     <hyperlink ref="F218" r:id="rId216" display="https://doi.org/10.1371/journal.pone.0298788"/>
     <hyperlink ref="F219" r:id="rId217" display="https://doi.org/10.1371/journal.pone.0298788"/>
+    <hyperlink ref="F220" r:id="rId218" display="https://doi.org/10.1371/journal.pone.0298788"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>